<commit_message>
Added Burn, Freeze and Paralyzed
</commit_message>
<xml_diff>
--- a/02_Requirements/Userstories.xlsx
+++ b/02_Requirements/Userstories.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DD1709-ACC5-41B5-AC43-7E30D7E41150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,9 +29,6 @@
     <t>As a player I want to change the games difficulty to my own liking</t>
   </si>
   <si>
-    <t>As a player I want my party to get stronger as i progress through the game</t>
-  </si>
-  <si>
     <t>As a player I want to see details about a move</t>
   </si>
   <si>
@@ -61,9 +59,6 @@
     <t>As a player I want the shield mechanic to increase the battles difficulty and make them more fun and unique</t>
   </si>
   <si>
-    <t>As a player I want the soulbar mechanik to make myself and the enemies stronger as well as provide interesting situations</t>
-  </si>
-  <si>
     <t>As a player I want to be able to use partner attacks to deal more damage</t>
   </si>
   <si>
@@ -79,9 +74,6 @@
     <t>As a player I want the game to teach me how to play it</t>
   </si>
   <si>
-    <t>As a player I want to choose my characters properties at the beginnig of the game</t>
-  </si>
-  <si>
     <t>As a player I want to be able to interact with the people and objects in the world</t>
   </si>
   <si>
@@ -95,13 +87,22 @@
   </si>
   <si>
     <t>As a player I want to be able to unlock new attacks as I progress through the game</t>
+  </si>
+  <si>
+    <t>As a player I want my party to get stronger as I progress through the game</t>
+  </si>
+  <si>
+    <t>As a player I want the soulbar mechanic to make myself and the enemies stronger as well as provide interesting situations</t>
+  </si>
+  <si>
+    <t>As a player I want to choose my characters properties at the beginning of the game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,13 +162,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -205,9 +214,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,9 +248,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -273,9 +300,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -448,19 +493,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="146" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,26 +513,29 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -495,7 +543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -503,161 +551,173 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>6</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
       <c r="C22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
       </c>
       <c r="C25">
         <v>2</v>

</xml_diff>

<commit_message>
added ids to our user stories
</commit_message>
<xml_diff>
--- a/02_Requirements/Userstories.xlsx
+++ b/02_Requirements/Userstories.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DD1709-ACC5-41B5-AC43-7E30D7E41150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -32,9 +31,6 @@
     <t>As a player I want to see details about a move</t>
   </si>
   <si>
-    <t>As a player I want to have in overworld with interesting locations to explore</t>
-  </si>
-  <si>
     <t>As a player I want to see my Health and Mana as well as the enemies</t>
   </si>
   <si>
@@ -96,13 +92,16 @@
   </si>
   <si>
     <t>As a player I want to choose my characters properties at the beginning of the game</t>
+  </si>
+  <si>
+    <t>As a player I want to have an overworld with interesting locations to explore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -214,9 +213,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,27 +247,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,27 +281,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,19 +456,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="146" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,217 +476,277 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
+      <c r="B23">
+        <v>22</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
       </c>
       <c r="C24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
         <v>5</v>
       </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C25">
+    <sortCondition ref="B2:B25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>